<commit_message>
Updated ERD and Normalization
</commit_message>
<xml_diff>
--- a/SQL/Normalization.xlsx
+++ b/SQL/Normalization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\331\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahma\Downloads\SQL 2\Project\fall2023database2project\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08E3A6A0-A6C3-4879-A28C-51B06FE3BA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A533CD4-7EA2-4C46-A10E-4C62718E44BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{1296AB01-AD24-4F16-91A3-E8FD79BCC2E7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{1296AB01-AD24-4F16-91A3-E8FD79BCC2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="UNF" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="178">
   <si>
     <t>customer firstname</t>
   </si>
@@ -581,7 +581,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,6 +779,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -938,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -994,9 +1009,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1008,6 +1020,11 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1259,10 +1276,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1568,25 +1581,25 @@
       <selection activeCell="D29" sqref="D29:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.5546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="27.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" customWidth="1"/>
     <col min="17" max="17" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -1668,7 +1681,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1707,7 +1720,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1746,7 +1759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1798,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>69</v>
       </c>
@@ -1820,7 +1833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
@@ -1853,7 +1866,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>36</v>
       </c>
@@ -1894,7 +1907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>76</v>
       </c>
@@ -1931,7 +1944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -1972,7 +1985,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
@@ -2013,7 +2026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -2095,7 +2108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -2136,7 +2149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -2173,7 +2186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2227,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
@@ -2255,7 +2268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -2294,7 +2307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>29</v>
       </c>
@@ -2335,7 +2348,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -2372,7 +2385,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
@@ -2409,7 +2422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>99</v>
       </c>
@@ -2444,7 +2457,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>93</v>
       </c>
@@ -2481,7 +2494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
@@ -2518,44 +2531,44 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="41"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-    </row>
-    <row r="28" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+    </row>
+    <row r="28" spans="1:22" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>107</v>
       </c>
@@ -2568,25 +2581,25 @@
       <c r="D28" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-    </row>
-    <row r="29" spans="1:22" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+    </row>
+    <row r="29" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>110</v>
       </c>
@@ -2600,7 +2613,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>112</v>
       </c>
@@ -2614,7 +2627,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>114</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>116</v>
       </c>
@@ -2642,7 +2655,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>118</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>120</v>
       </c>
@@ -2670,7 +2683,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>110</v>
       </c>
@@ -2684,7 +2697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>110</v>
       </c>
@@ -2698,7 +2711,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>118</v>
       </c>
@@ -2712,7 +2725,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>120</v>
       </c>
@@ -2726,7 +2739,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>114</v>
       </c>
@@ -2740,7 +2753,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>112</v>
       </c>
@@ -2754,7 +2767,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>116</v>
       </c>
@@ -2768,7 +2781,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>118</v>
       </c>
@@ -2782,7 +2795,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>120</v>
       </c>
@@ -2796,7 +2809,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>110</v>
       </c>
@@ -2810,7 +2823,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
         <v>116</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="18" t="s">
         <v>110</v>
       </c>
@@ -2838,7 +2851,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>118</v>
       </c>
@@ -2898,30 +2911,30 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2940,7 +2953,7 @@
       <c r="F1" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>136</v>
       </c>
       <c r="H1" s="25" t="s">
@@ -2970,7 +2983,7 @@
       <c r="P1" s="33"/>
       <c r="T1" s="23"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3008,7 +3021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3046,7 +3059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3093,7 +3106,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3134,7 +3147,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3181,12 +3194,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="43" t="s">
         <v>152</v>
       </c>
       <c r="C11" t="s">
@@ -3202,14 +3215,14 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>154</v>
       </c>
       <c r="C12">
         <v>350</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>168</v>
       </c>
       <c r="E12" t="s">
@@ -3219,14 +3232,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>112</v>
       </c>
       <c r="C13">
         <v>1000</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>169</v>
       </c>
       <c r="E13" t="s">
@@ -3236,14 +3249,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>114</v>
       </c>
       <c r="C14">
         <v>80</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>171</v>
       </c>
       <c r="E14" t="s">
@@ -3253,14 +3266,14 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>114</v>
       </c>
       <c r="C15">
         <v>200</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="41" t="s">
         <v>173</v>
       </c>
       <c r="E15" t="s">
@@ -3270,14 +3283,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>116</v>
       </c>
       <c r="C16">
         <v>200</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>175</v>
       </c>
       <c r="E16" t="s">
@@ -3287,7 +3300,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>164</v>
       </c>
@@ -3303,25 +3316,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25792CA2-A340-4818-8933-963BC1F39245}">
   <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
     <col min="16" max="16" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -3341,7 +3354,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3358,7 +3371,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -3375,7 +3388,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3395,7 +3408,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3415,7 +3428,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>136</v>
       </c>
@@ -3425,7 +3438,7 @@
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>80</v>
       </c>
@@ -3448,7 +3461,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>48</v>
       </c>
@@ -3471,7 +3484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>81</v>
       </c>
@@ -3494,7 +3507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>80</v>
       </c>
@@ -3517,7 +3530,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>81</v>
       </c>
@@ -3540,7 +3553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G15" s="24">
         <v>45206</v>
       </c>
@@ -3557,11 +3570,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E17" s="33"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
         <v>152</v>
       </c>
       <c r="B25" t="s">
@@ -3580,14 +3593,14 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>154</v>
       </c>
       <c r="B26">
         <v>350</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>168</v>
       </c>
       <c r="D26" t="s">
@@ -3612,14 +3625,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>112</v>
       </c>
       <c r="B27">
         <v>1000</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="41" t="s">
         <v>169</v>
       </c>
       <c r="D27" t="s">
@@ -3641,14 +3654,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
       <c r="B28">
         <v>80</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="41" t="s">
         <v>171</v>
       </c>
       <c r="D28" t="s">
@@ -3670,14 +3683,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
       <c r="B29">
         <v>200</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="41" t="s">
         <v>173</v>
       </c>
       <c r="D29" t="s">
@@ -3702,14 +3715,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>116</v>
       </c>
       <c r="B30">
         <v>200</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="41" t="s">
         <v>175</v>
       </c>
       <c r="D30" t="s">
@@ -3731,7 +3744,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>1</v>
       </c>
@@ -3742,38 +3755,38 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -3790,23 +3803,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39EB8510-681A-434A-8FF2-0CFA5EDA1D1E}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -3821,21 +3836,21 @@
       </c>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="44" t="s">
         <v>127</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>126</v>
       </c>
       <c r="K1" s="22"/>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="44" t="s">
         <v>126</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3855,7 +3870,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3875,7 +3890,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3901,7 +3916,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3927,7 +3942,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>136</v>
       </c>
@@ -3937,7 +3952,7 @@
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>80</v>
       </c>
@@ -3953,14 +3968,14 @@
       <c r="I9" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="42" t="s">
         <v>136</v>
       </c>
       <c r="K9" s="32" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>48</v>
       </c>
@@ -3983,7 +3998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="24" t="s">
         <v>81</v>
       </c>
@@ -4006,7 +4021,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>80</v>
       </c>
@@ -4029,7 +4044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>81</v>
       </c>
@@ -4052,7 +4067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G14" s="24">
         <v>45206</v>
       </c>
@@ -4069,11 +4084,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E16" s="33"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>152</v>
       </c>
       <c r="B24" t="s">
@@ -4082,45 +4097,48 @@
       <c r="C24" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="42" t="s">
         <v>136</v>
       </c>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>154</v>
       </c>
       <c r="B25">
         <v>350</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="41" t="s">
         <v>168</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>80</v>
       </c>
+      <c r="G25" s="52" t="s">
+        <v>141</v>
+      </c>
       <c r="H25" s="26" t="s">
         <v>140</v>
       </c>
       <c r="I25" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="J25" s="43" t="s">
+      <c r="J25" s="42" t="s">
         <v>136</v>
       </c>
       <c r="K25" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>112</v>
       </c>
       <c r="B26">
         <v>1000</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>169</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -4136,14 +4154,14 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>114</v>
       </c>
       <c r="B27">
         <v>80</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="41" t="s">
         <v>171</v>
       </c>
       <c r="D27" s="24" t="s">
@@ -4159,14 +4177,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
       <c r="B28">
         <v>200</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="41" t="s">
         <v>173</v>
       </c>
       <c r="D28" s="24" t="s">
@@ -4185,14 +4203,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>116</v>
       </c>
       <c r="B29">
         <v>200</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="41" t="s">
         <v>175</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -4208,7 +4226,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>1</v>
       </c>
@@ -4219,38 +4237,38 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -4267,23 +4285,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD3E6DA-A7F9-43D6-91D3-99B6F522048C}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>158</v>
       </c>
@@ -4299,26 +4317,26 @@
       <c r="E1" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>127</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="45" t="s">
         <v>126</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>76</v>
       </c>
@@ -4341,7 +4359,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -4393,7 +4411,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -4422,8 +4440,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
         <v>145</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -4444,14 +4462,14 @@
       <c r="I8" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="48" t="s">
         <v>145</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
         <v>80</v>
       </c>
@@ -4468,7 +4486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
         <v>48</v>
       </c>
@@ -4485,7 +4503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="24" t="s">
         <v>81</v>
       </c>
@@ -4502,7 +4520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
         <v>80</v>
       </c>
@@ -4519,7 +4537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
         <v>81</v>
       </c>
@@ -4536,20 +4554,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>153</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="48" t="s">
         <v>145</v>
       </c>
       <c r="H17" s="32" t="s">
@@ -4559,7 +4577,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>154</v>
       </c>
@@ -4570,7 +4588,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>112</v>
       </c>
@@ -4581,7 +4599,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>114</v>
       </c>
@@ -4592,7 +4610,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>114</v>
       </c>
@@ -4603,7 +4621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>116</v>
       </c>
@@ -4614,7 +4632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -4624,29 +4642,31 @@
       <c r="C25" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="49" t="s">
-        <v>145</v>
+      <c r="D25" s="52" t="s">
+        <v>141</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>4</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>3</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>1</v>
       </c>
@@ -4656,14 +4676,14 @@
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>4</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1</v>
       </c>
@@ -4685,29 +4705,29 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>155</v>
       </c>
       <c r="G1" s="38"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>124</v>
       </c>
@@ -4729,7 +4749,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4746,7 +4766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4763,7 +4783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4780,7 +4800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4797,7 +4817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>108</v>
       </c>
@@ -4805,7 +4825,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>145</v>
       </c>
@@ -4837,7 +4857,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4869,7 +4889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -4901,7 +4921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -4933,7 +4953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4965,7 +4985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -4997,7 +5017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
         <v>160</v>
       </c>
@@ -5005,7 +5025,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>139</v>
       </c>
@@ -5028,7 +5048,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5045,7 +5065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -5062,7 +5082,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -5085,7 +5105,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -5102,7 +5122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -5125,13 +5145,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>162</v>
       </c>
       <c r="G24" s="38"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
         <v>151</v>
       </c>
@@ -5147,7 +5167,7 @@
       <c r="G25" s="23"/>
       <c r="H25" s="30"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -5155,7 +5175,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -5163,7 +5183,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -5171,7 +5191,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -5179,7 +5199,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -5187,12 +5207,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="38" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>156</v>
       </c>
@@ -5206,7 +5226,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -5223,7 +5243,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -5240,7 +5260,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3</v>
       </c>
@@ -5260,7 +5280,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -5280,7 +5300,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G42">
         <v>4</v>
       </c>
@@ -5291,17 +5311,17 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="41" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5313,6 +5333,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006906BD691B85264BAE92BBA364CF27E7" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f2fd7e278f3424424cf8cae7e3fca23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="71c21392-2f97-4640-aa4b-3df5c4132913" xmlns:ns4="95d96561-6f8f-4900-8a68-84dfb5dc8926" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6de66d2a75c7fcabe8ddbb0cbdbe162f" ns3:_="" ns4:_="">
     <xsd:import namespace="71c21392-2f97-4640-aa4b-3df5c4132913"/>
@@ -5509,15 +5538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5527,6 +5547,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{804FD600-E57E-442F-A034-EF32490E5506}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46BC4315-00C2-4338-925A-FFBBEAB637D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5541,14 +5569,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{804FD600-E57E-442F-A034-EF32490E5506}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>